<commit_message>
Added officer to xlxs
Cottage - ad15
</commit_message>
<xml_diff>
--- a/officer netids.xlsx
+++ b/officer netids.xlsx
@@ -1,23 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="27426"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ben\Documents\GitHub\Prospective\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yangtu/Documents/Pton/COS/COS 333/proj/Prospective/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C6130902-AAE8-443C-8DE7-8947652D3F6F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" xr2:uid="{6AB3F543-C7DB-4BA8-8FCC-79860E79363E}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="23040" windowHeight="9080"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="46">
   <si>
     <t>Cannon</t>
   </si>
@@ -168,7 +173,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -513,29 +518,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6CB0B2D-9BCA-4BAE-84F7-9BA6E157E8CF}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.77734375" customWidth="1"/>
-    <col min="2" max="2" width="17.77734375" customWidth="1"/>
+    <col min="1" max="1" width="16.83203125" customWidth="1"/>
+    <col min="2" max="2" width="17.83203125" customWidth="1"/>
     <col min="3" max="3" width="13.6640625" customWidth="1"/>
     <col min="4" max="4" width="14.6640625" customWidth="1"/>
-    <col min="5" max="5" width="17.44140625" customWidth="1"/>
+    <col min="5" max="5" width="17.5" customWidth="1"/>
     <col min="6" max="6" width="13.6640625" customWidth="1"/>
-    <col min="7" max="7" width="17.21875" customWidth="1"/>
+    <col min="7" max="7" width="17.1640625" customWidth="1"/>
     <col min="8" max="8" width="13.33203125" customWidth="1"/>
-    <col min="9" max="9" width="17.5546875" customWidth="1"/>
-    <col min="10" max="10" width="14.88671875" customWidth="1"/>
-    <col min="11" max="11" width="15.77734375" customWidth="1"/>
+    <col min="9" max="9" width="17.5" customWidth="1"/>
+    <col min="10" max="10" width="14.83203125" customWidth="1"/>
+    <col min="11" max="11" width="15.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -570,7 +575,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -586,6 +591,9 @@
       <c r="E2" t="s">
         <v>25</v>
       </c>
+      <c r="F2" t="s">
+        <v>12</v>
+      </c>
       <c r="G2" t="s">
         <v>30</v>
       </c>
@@ -602,7 +610,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -634,7 +642,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -666,7 +674,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -677,7 +685,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>15</v>
       </c>

</xml_diff>